<commit_message>
Add expected output format documentation in "README.md"
</commit_message>
<xml_diff>
--- a/output_example_v1.xlsx
+++ b/output_example_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitigronbunyakunjarean/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tee4cute/Programming/source/thailand-budget-pdf2csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048A6534-1DC1-8D4E-8A38-2C74A145A2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49DAFD5A-CD5D-8F4B-BB0B-F254FBEB37F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4600" yWindow="-20500" windowWidth="38040" windowHeight="16960" activeTab="1" xr2:uid="{98AA100D-2A38-7F43-B940-F6FBE4CFE11C}"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{98AA100D-2A38-7F43-B940-F6FBE4CFE11C}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -230,9 +239,6 @@
     <t>โครงการ</t>
   </si>
   <si>
-    <t>บางแผนงาน ไม่มีผลผลิต AND ไม่มีโครงการ, 1 รายการ สามารถอยู่ได้เพียง 1 แผนงาน XOR 1 โครงการ อย่างใดอย่างหนึ่ง</t>
-  </si>
-  <si>
     <t>หมวดงบประมาณ lvl.1, ทุกรายการ ต้องมีอย่างน้อย lvl.1</t>
   </si>
   <si>
@@ -270,6 +276,9 @@
   </si>
   <si>
     <t>มีโอกาสที่รายการจะมีหลาย row FISCAL_YEAR ได้ ถ้ารายการนั้น เป็นรายการงบผูกพัน</t>
+  </si>
+  <si>
+    <t>บางแผนงาน ไม่มีผลผลิต AND ไม่มีโครงการ, 1 รายการ สามารถอยู่ได้เพียง 1 ผลผลิต XOR 1 โครงการ อย่างใดอย่างหนึ่ง</t>
   </si>
 </sst>
 </file>
@@ -738,7 +747,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1311,7 +1320,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1328,7 @@
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="110.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1327,7 +1336,7 @@
         <v>41</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>43</v>
@@ -1421,7 +1430,7 @@
         <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1432,7 +1441,7 @@
         <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1440,7 +1449,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1448,7 +1457,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1456,7 +1465,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1464,7 +1473,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1472,7 +1481,7 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1480,7 +1489,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1488,7 +1497,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1496,10 +1505,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1507,7 +1516,7 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1515,13 +1524,13 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
         <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7643E4EB-94B5-E449-9FE7-38737EE20297}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="66" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="75" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix wrong output example in xlsx file.
</commit_message>
<xml_diff>
--- a/output_example_v1.xlsx
+++ b/output_example_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tee4cute/Programming/source/thailand-budget-pdf2csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49DAFD5A-CD5D-8F4B-BB0B-F254FBEB37F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DF680D-9A39-624D-A607-5C0C9ABA0F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{98AA100D-2A38-7F43-B940-F6FBE4CFE11C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" xr2:uid="{98AA100D-2A38-7F43-B940-F6FBE4CFE11C}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="81">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9123105-0E0A-AA42-A417-FB07BE8F7050}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,9 +896,6 @@
         <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="Q3" s="1">
@@ -1319,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71F3066-2353-0647-9580-39C183103A38}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>